<commit_message>
fix PR comments: add phone number and other template data, fix hashmap etc
</commit_message>
<xml_diff>
--- a/src/test/resources/data/SheetTemplate.xlsx
+++ b/src/test/resources/data/SheetTemplate.xlsx
@@ -34,10 +34,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>real phone number</t>
-  </si>
-  <si>
-    <t>your name</t>
+    <t>password from your mzgb account</t>
   </si>
   <si>
     <t>name of your team</t>
@@ -46,10 +43,13 @@
     <t>number of players</t>
   </si>
   <si>
-    <t>password from your mzgb account</t>
-  </si>
-  <si>
-    <t>your real email</t>
+    <t>John</t>
+  </si>
+  <si>
+    <t>john@test.com</t>
+  </si>
+  <si>
+    <t>+48521439678</t>
   </si>
 </sst>
 </file>
@@ -94,9 +94,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -405,13 +408,13 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -419,24 +422,24 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -444,8 +447,8 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -453,7 +456,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -461,11 +464,17 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>